<commit_message>
2021_02_07 on mobile lynuxx_cmds.xlsx changes
</commit_message>
<xml_diff>
--- a/lynux_cmds.xlsx
+++ b/lynux_cmds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_WORK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F462CAB-F9ED-D448-A3B6-8AB28D07A84A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{EB371ED8-065F-C34E-A6A9-39266BDF1A70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="2295" windowWidth="16245" windowHeight="12705" xr2:uid="{8F2625FD-89A9-4B3D-8A00-8DF7F9DA0750}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Notes</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t xml:space="preserve"> je tzv. prototyp mountovania</t>
+  </si>
+  <si>
+    <t>sudo fdisk -l</t>
+  </si>
+  <si>
+    <t>vypis diskov v systeme</t>
   </si>
 </sst>
 </file>
@@ -647,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDC9B31-712E-4E5B-94AD-D272F284797C}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -942,6 +948,14 @@
         <v>68</v>
       </c>
     </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{5C62FD82-4872-4EC9-A92A-846A76165160}"/>

</xml_diff>

<commit_message>
2021_03_22 - termux commnads update
</commit_message>
<xml_diff>
--- a/lynux_cmds.xlsx
+++ b/lynux_cmds.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_WORK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\_WORK\PYTHON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{8F8A72B4-0592-5044-BF9F-F1266C9792CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2453FA-9429-48B8-A621-C47197E2D07E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="2295" windowWidth="16245" windowHeight="12705" xr2:uid="{8F2625FD-89A9-4B3D-8A00-8DF7F9DA0750}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{8F2625FD-89A9-4B3D-8A00-8DF7F9DA0750}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="Termux cmds" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -26,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="290">
   <si>
     <t>Notes</t>
   </si>
@@ -308,13 +308,610 @@
   </si>
   <si>
     <t>po zruseni kopirovania bude mat 10 pokusov na obnovenie</t>
+  </si>
+  <si>
+    <t>COMMANDS</t>
+  </si>
+  <si>
+    <t>USAGE</t>
+  </si>
+  <si>
+    <t>cp -v</t>
+  </si>
+  <si>
+    <t>used to prints informative massage</t>
+  </si>
+  <si>
+    <t>cp -r</t>
+  </si>
+  <si>
+    <t>used to copy any directory</t>
+  </si>
+  <si>
+    <t>mv -u</t>
+  </si>
+  <si>
+    <t>update-move when source is newer than destination</t>
+  </si>
+  <si>
+    <t>mv -v</t>
+  </si>
+  <si>
+    <t>to move any directory</t>
+  </si>
+  <si>
+    <t>ls -n</t>
+  </si>
+  <si>
+    <t>to display UID and GID directory</t>
+  </si>
+  <si>
+    <t>ls --version</t>
+  </si>
+  <si>
+    <t>to check the version of ls command</t>
+  </si>
+  <si>
+    <t>cd --</t>
+  </si>
+  <si>
+    <t>show last working directory from where we moved</t>
+  </si>
+  <si>
+    <t>ls -l</t>
+  </si>
+  <si>
+    <t>show file action like - modified, date and time, owner of file, permissions Etc.</t>
+  </si>
+  <si>
+    <t>ls help</t>
+  </si>
+  <si>
+    <t>show display how to use "ls" command</t>
+  </si>
+  <si>
+    <t>cp -n</t>
+  </si>
+  <si>
+    <t>no file overwrite</t>
+  </si>
+  <si>
+    <t>cd ~</t>
+  </si>
+  <si>
+    <t>move to users home directory from anywhere</t>
+  </si>
+  <si>
+    <t>mv [file1 name] [new file2 name]</t>
+  </si>
+  <si>
+    <t>move or rename two file at a time</t>
+  </si>
+  <si>
+    <t>cd -</t>
+  </si>
+  <si>
+    <t>move one directory back from current location</t>
+  </si>
+  <si>
+    <t>mv [file name]</t>
+  </si>
+  <si>
+    <t>move any file and folder</t>
+  </si>
+  <si>
+    <t>ls</t>
+  </si>
+  <si>
+    <t>list directory</t>
+  </si>
+  <si>
+    <t>ls -a</t>
+  </si>
+  <si>
+    <t>list all files including hidden files</t>
+  </si>
+  <si>
+    <t>it show your current working directory</t>
+  </si>
+  <si>
+    <t>mv -i</t>
+  </si>
+  <si>
+    <t>interactive prompt before overwrit</t>
+  </si>
+  <si>
+    <t>wget [url]</t>
+  </si>
+  <si>
+    <t>install tool , apt install wget</t>
+  </si>
+  <si>
+    <t>git clone [url]</t>
+  </si>
+  <si>
+    <t>install any tools with git clone, apt install git</t>
+  </si>
+  <si>
+    <t>ls -al</t>
+  </si>
+  <si>
+    <t>formatted listing with hidden files</t>
+  </si>
+  <si>
+    <t>mv -f</t>
+  </si>
+  <si>
+    <t>force move by overwriting destination files without prompt</t>
+  </si>
+  <si>
+    <t>ls -i</t>
+  </si>
+  <si>
+    <t>Display number of file or directory</t>
+  </si>
+  <si>
+    <t>cp</t>
+  </si>
+  <si>
+    <t>copy any file</t>
+  </si>
+  <si>
+    <t>cd /</t>
+  </si>
+  <si>
+    <t>change to root directory</t>
+  </si>
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>change directory</t>
+  </si>
+  <si>
+    <t>cd ..</t>
+  </si>
+  <si>
+    <t>change current directory to parent directory</t>
+  </si>
+  <si>
+    <t>curl -O [url]</t>
+  </si>
+  <si>
+    <t>apt install curl</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>remove or delete files</t>
+  </si>
+  <si>
+    <t>rm [filename]</t>
+  </si>
+  <si>
+    <t>remove any text files</t>
+  </si>
+  <si>
+    <t>rmdir [dir name]</t>
+  </si>
+  <si>
+    <t>remove any directory</t>
+  </si>
+  <si>
+    <t>rm -rf</t>
+  </si>
+  <si>
+    <t>force remove a directory or a folder</t>
+  </si>
+  <si>
+    <t>rm -r [name]</t>
+  </si>
+  <si>
+    <t>delete a directory called name</t>
+  </si>
+  <si>
+    <t>apt remove [package name]</t>
+  </si>
+  <si>
+    <t>uninstall / remove a package</t>
+  </si>
+  <si>
+    <t>touch [file name]</t>
+  </si>
+  <si>
+    <t>create new file</t>
+  </si>
+  <si>
+    <t>mkdir [name]</t>
+  </si>
+  <si>
+    <t>create a directory or folder</t>
+  </si>
+  <si>
+    <t>more [file name]</t>
+  </si>
+  <si>
+    <t>output the contents of file</t>
+  </si>
+  <si>
+    <t>head [file name]</t>
+  </si>
+  <si>
+    <t>output the first 10 line of file</t>
+  </si>
+  <si>
+    <t>tail -f [file name]</t>
+  </si>
+  <si>
+    <t>output the contents of file as it grows</t>
+  </si>
+  <si>
+    <t>apt install zip</t>
+  </si>
+  <si>
+    <t>install zip file tool</t>
+  </si>
+  <si>
+    <t>zip name.zip [file]</t>
+  </si>
+  <si>
+    <t>compress file using this commands</t>
+  </si>
+  <si>
+    <t>unzip [zip file]</t>
+  </si>
+  <si>
+    <t>to unzip file</t>
+  </si>
+  <si>
+    <t>ftp</t>
+  </si>
+  <si>
+    <t>launch ftp client from terminal</t>
+  </si>
+  <si>
+    <t>-p</t>
+  </si>
+  <si>
+    <t>use passive mode</t>
+  </si>
+  <si>
+    <t>bye</t>
+  </si>
+  <si>
+    <t>terminate current ftp session, exit</t>
+  </si>
+  <si>
+    <t>ascii</t>
+  </si>
+  <si>
+    <t>set file transfer to ascii protocols</t>
+  </si>
+  <si>
+    <t>bell</t>
+  </si>
+  <si>
+    <t>bell sound after each command</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>shows current status about ftp server</t>
+  </si>
+  <si>
+    <t>open host</t>
+  </si>
+  <si>
+    <t>open a connection to remote host</t>
+  </si>
+  <si>
+    <t>remotehelp [cmdname]</t>
+  </si>
+  <si>
+    <t>request help from ftp server</t>
+  </si>
+  <si>
+    <t>account [password]</t>
+  </si>
+  <si>
+    <t>supply a password required by remote</t>
+  </si>
+  <si>
+    <t>uname -m</t>
+  </si>
+  <si>
+    <t>used to find the architecture of your device</t>
+  </si>
+  <si>
+    <t>du</t>
+  </si>
+  <si>
+    <t>display directory space usage</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>display disk usages</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>show display calendar</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>show display who is currently online</t>
+  </si>
+  <si>
+    <t>cat /proc/meminfo</t>
+  </si>
+  <si>
+    <t>show memory related information</t>
+  </si>
+  <si>
+    <t>cat /proc/cpuinfo</t>
+  </si>
+  <si>
+    <t>show cpu information</t>
+  </si>
+  <si>
+    <t>whoami</t>
+  </si>
+  <si>
+    <t>show your login name</t>
+  </si>
+  <si>
+    <t>fingure username</t>
+  </si>
+  <si>
+    <t>shows information about user</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>show the current date and time</t>
+  </si>
+  <si>
+    <t>uptime</t>
+  </si>
+  <si>
+    <t>show the system current uptime</t>
+  </si>
+  <si>
+    <t>man command</t>
+  </si>
+  <si>
+    <t>show manual a command</t>
+  </si>
+  <si>
+    <t>free</t>
+  </si>
+  <si>
+    <t>display memory and swap usage</t>
+  </si>
+  <si>
+    <t>kill</t>
+  </si>
+  <si>
+    <t>send signal to process</t>
+  </si>
+  <si>
+    <t>kill- l</t>
+  </si>
+  <si>
+    <t>list all of the signal that are possible to send with kill</t>
+  </si>
+  <si>
+    <t>lspci</t>
+  </si>
+  <si>
+    <t>show PCI devices</t>
+  </si>
+  <si>
+    <t>lsusb</t>
+  </si>
+  <si>
+    <t>show usb devices</t>
+  </si>
+  <si>
+    <t>apt search [qurey]</t>
+  </si>
+  <si>
+    <t>pkg search [qurey]</t>
+  </si>
+  <si>
+    <t>find a package</t>
+  </si>
+  <si>
+    <t>locate [file]</t>
+  </si>
+  <si>
+    <t>find all files with filename</t>
+  </si>
+  <si>
+    <t>locate [query]</t>
+  </si>
+  <si>
+    <t>find all path names contains a pharse</t>
+  </si>
+  <si>
+    <t>whereis [command]</t>
+  </si>
+  <si>
+    <t>find location binary /source/man file for a command</t>
+  </si>
+  <si>
+    <t>which [command]</t>
+  </si>
+  <si>
+    <t>find of an executable</t>
+  </si>
+  <si>
+    <t>grep pattern [files]</t>
+  </si>
+  <si>
+    <t>searching for pattern in files</t>
+  </si>
+  <si>
+    <t>grep -r pattern files</t>
+  </si>
+  <si>
+    <t>searching for certain pattern in files</t>
+  </si>
+  <si>
+    <t>command | grep pattern</t>
+  </si>
+  <si>
+    <t>search for pattern in the output of command</t>
+  </si>
+  <si>
+    <t>find / -atime40</t>
+  </si>
+  <si>
+    <t>to find all the files, which are accessed 40 days back</t>
+  </si>
+  <si>
+    <t>find / -cmin -60</t>
+  </si>
+  <si>
+    <t>find change files in last 1 hour</t>
+  </si>
+  <si>
+    <t>find / -type d -name mll</t>
+  </si>
+  <si>
+    <t>find all directories whose name is mll in directory</t>
+  </si>
+  <si>
+    <t>find . -type f -perm 0777 -print</t>
+  </si>
+  <si>
+    <t>find all tghe files, whose permission are 777</t>
+  </si>
+  <si>
+    <t>ifconfig</t>
+  </si>
+  <si>
+    <t>shows all configuration a network interface like ip, mac</t>
+  </si>
+  <si>
+    <t>ifconfig eth0</t>
+  </si>
+  <si>
+    <t>used view the network setting on the interface eth0</t>
+  </si>
+  <si>
+    <t>ifconfig wlan0</t>
+  </si>
+  <si>
+    <t>view the network setting on wlan0</t>
+  </si>
+  <si>
+    <t>ping [host]</t>
+  </si>
+  <si>
+    <t>to ping host ip and show results</t>
+  </si>
+  <si>
+    <t>arp</t>
+  </si>
+  <si>
+    <t>check network card &amp; show ip adress</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>display specific server</t>
+  </si>
+  <si>
+    <t>netstat</t>
+  </si>
+  <si>
+    <t>review network connection</t>
+  </si>
+  <si>
+    <t>nslookup</t>
+  </si>
+  <si>
+    <t>find out DNS related query</t>
+  </si>
+  <si>
+    <t>tracerout ipadress</t>
+  </si>
+  <si>
+    <t>display number of hops &amp; respone time to get to a remote system and website</t>
+  </si>
+  <si>
+    <t>whois domain</t>
+  </si>
+  <si>
+    <t>get whois information of domain</t>
+  </si>
+  <si>
+    <t>telnet [ip address [post]</t>
+  </si>
+  <si>
+    <t>telnet connection</t>
+  </si>
+  <si>
+    <t>dig domain</t>
+  </si>
+  <si>
+    <t>get DNS information of domain</t>
+  </si>
+  <si>
+    <t>scp</t>
+  </si>
+  <si>
+    <t>copies file, over a source</t>
+  </si>
+  <si>
+    <t>used to display kernal information</t>
+  </si>
+  <si>
+    <t>whereis app</t>
+  </si>
+  <si>
+    <t>shows possible location for an app</t>
+  </si>
+  <si>
+    <t>nano [file name]</t>
+  </si>
+  <si>
+    <t>display and edit text files</t>
+  </si>
+  <si>
+    <t>apt show</t>
+  </si>
+  <si>
+    <t>view package information</t>
+  </si>
+  <si>
+    <t>append [local-file] remote file</t>
+  </si>
+  <si>
+    <t>append a local file to one on the remote</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>execute a macro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,8 +948,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,8 +979,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -386,12 +1006,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -402,10 +1040,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hypertextové prepojenie" xfId="1" builtinId="8"/>
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -421,7 +1078,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív balíka Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -719,18 +1376,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDC9B31-712E-4E5B-94AD-D272F284797C}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.4140625" customWidth="1"/>
-    <col min="3" max="3" width="44.2578125" customWidth="1"/>
+    <col min="1" max="1" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -741,8 +1398,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="6" customFormat="1"/>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -750,7 +1407,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -759,7 +1416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="5" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -767,7 +1424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" s="5" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -775,7 +1432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="5" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -783,7 +1440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="5" customFormat="1">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -791,7 +1448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="5" customFormat="1">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -799,7 +1456,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -807,12 +1464,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="5" customFormat="1">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="5" customFormat="1">
       <c r="A12" s="5" t="s">
         <v>75</v>
       </c>
@@ -823,7 +1480,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="5" customFormat="1">
       <c r="A13" s="5" t="s">
         <v>78</v>
       </c>
@@ -831,7 +1488,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="5" customFormat="1">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -839,12 +1496,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="5" customFormat="1">
       <c r="A15" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="5" customFormat="1">
       <c r="A16" s="5" t="s">
         <v>55</v>
       </c>
@@ -852,7 +1509,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="5" customFormat="1">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
@@ -860,7 +1517,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -868,7 +1525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -876,12 +1533,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -889,7 +1546,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -897,7 +1554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -905,7 +1562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -913,7 +1570,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -921,7 +1578,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -929,7 +1586,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -937,7 +1594,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -945,7 +1602,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -953,7 +1610,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -961,7 +1618,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -969,7 +1626,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="1" customFormat="1">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -978,12 +1635,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="3" customFormat="1">
       <c r="A33" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="3" customFormat="1">
       <c r="A34" s="3" t="s">
         <v>82</v>
       </c>
@@ -991,7 +1648,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="3" customFormat="1">
       <c r="A35" s="3" t="s">
         <v>61</v>
       </c>
@@ -999,15 +1656,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" s="3" customFormat="1"/>
+    <row r="37" spans="1:3" s="1" customFormat="1">
       <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -1015,7 +1672,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -1023,14 +1680,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="1" customFormat="1">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1041,7 +1698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -1049,7 +1706,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>65</v>
       </c>
@@ -1057,7 +1714,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="43.2">
       <c r="A45" s="7" t="s">
         <v>89</v>
       </c>
@@ -1065,7 +1722,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -1073,7 +1730,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -1081,7 +1738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -1089,7 +1746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -1097,7 +1754,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -1113,4 +1770,841 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B050774F-0248-4535-9BF1-60C62C83C9E5}">
+  <dimension ref="A1:C101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="6" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="15" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1">
+      <c r="A3" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="6" customFormat="1" ht="15" thickBot="1">
+      <c r="A4" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1">
+      <c r="A5" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1">
+      <c r="A6" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1">
+      <c r="A7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1">
+      <c r="A8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="23.4" thickBot="1">
+      <c r="A9" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1">
+      <c r="A10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1">
+      <c r="A11" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1">
+      <c r="A12" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1">
+      <c r="A13" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1">
+      <c r="A14" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1">
+      <c r="A15" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1">
+      <c r="A16" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1">
+      <c r="A17" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1">
+      <c r="A18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1">
+      <c r="A19" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1">
+      <c r="A20" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1">
+      <c r="A21" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1">
+      <c r="A22" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="23.4" thickBot="1">
+      <c r="A23" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1">
+      <c r="A24" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1">
+      <c r="A25" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1">
+      <c r="A26" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1">
+      <c r="A27" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1">
+      <c r="A28" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1">
+      <c r="A29" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1">
+      <c r="A30" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1">
+      <c r="A31" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="6" customFormat="1" ht="15" thickBot="1">
+      <c r="A32" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1">
+      <c r="A33" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1">
+      <c r="A34" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1">
+      <c r="A35" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1">
+      <c r="A36" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="6" customFormat="1" ht="15" thickBot="1">
+      <c r="A37" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1">
+      <c r="A38" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" thickBot="1">
+      <c r="A39" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" thickBot="1">
+      <c r="A40" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="6" customFormat="1" ht="15" thickBot="1">
+      <c r="A41" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1">
+      <c r="A42" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1">
+      <c r="A43" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1">
+      <c r="A44" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" thickBot="1">
+      <c r="A45" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" thickBot="1">
+      <c r="A46" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" thickBot="1">
+      <c r="A47" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" thickBot="1">
+      <c r="A48" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1">
+      <c r="A49" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1">
+      <c r="A50" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1">
+      <c r="A51" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1">
+      <c r="A52" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1">
+      <c r="A53" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" thickBot="1">
+      <c r="A54" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1">
+      <c r="A55" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" thickBot="1">
+      <c r="A56" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" thickBot="1">
+      <c r="A57" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" thickBot="1">
+      <c r="A58" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1">
+      <c r="A59" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1">
+      <c r="A60" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" thickBot="1">
+      <c r="A61" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1">
+      <c r="A62" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" thickBot="1">
+      <c r="A63" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1">
+      <c r="A64" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" thickBot="1">
+      <c r="A65" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1">
+      <c r="A66" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15" thickBot="1">
+      <c r="A67" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15" thickBot="1">
+      <c r="A68" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15" thickBot="1">
+      <c r="A69" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" thickBot="1">
+      <c r="A71" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B71" s="13"/>
+    </row>
+    <row r="72" spans="1:2" ht="15" thickBot="1">
+      <c r="A72" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15" thickBot="1">
+      <c r="A73" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15" thickBot="1">
+      <c r="A74" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15" thickBot="1">
+      <c r="A75" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15" thickBot="1">
+      <c r="A76" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15" thickBot="1">
+      <c r="A77" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15" thickBot="1">
+      <c r="A78" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="23.4" thickBot="1">
+      <c r="A79" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15" thickBot="1">
+      <c r="A80" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15" thickBot="1">
+      <c r="A81" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15" thickBot="1">
+      <c r="A82" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="23.4" thickBot="1">
+      <c r="A83" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15" thickBot="1">
+      <c r="A84" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15" thickBot="1">
+      <c r="A85" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15" thickBot="1">
+      <c r="A86" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15" thickBot="1">
+      <c r="A87" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15" thickBot="1">
+      <c r="A88" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15" thickBot="1">
+      <c r="A89" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" thickBot="1">
+      <c r="A90" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="23.4" thickBot="1">
+      <c r="A91" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" thickBot="1">
+      <c r="A92" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" thickBot="1">
+      <c r="A93" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" thickBot="1">
+      <c r="A94" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" thickBot="1">
+      <c r="A95" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" thickBot="1">
+      <c r="A96" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" thickBot="1">
+      <c r="A97" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" thickBot="1">
+      <c r="A98" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15" thickBot="1">
+      <c r="A99" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15" thickBot="1">
+      <c r="A100" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>289</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B70:B71"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>